<commit_message>
Encoder drawing is started.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/IMMD Production/Encoder.xlsx
+++ b/Project/3501/Furkan/IMMD Production/Encoder.xlsx
@@ -66,21 +66,6 @@
     <t xml:space="preserve">http://www.alfasanayi.com/arc-h-50-hollow-saft-atek-made-in-turkey-urun-176.html </t>
   </si>
   <si>
-    <t>E80H30</t>
-  </si>
-  <si>
-    <t>80 mm</t>
-  </si>
-  <si>
-    <t>30 mm</t>
-  </si>
-  <si>
-    <t>3200 ppr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.turanmuhendislik.com.tr/e80h-serisi-enkoderler </t>
-  </si>
-  <si>
     <t>E40H8-2500-6-L-5</t>
   </si>
   <si>
@@ -100,6 +85,21 @@
   </si>
   <si>
     <t xml:space="preserve">http://www.endelkon.com/autonics-e40h8-25006-l-5-pmu1553 </t>
+  </si>
+  <si>
+    <t>Çıkış Tipi</t>
+  </si>
+  <si>
+    <t>Push Pull</t>
+  </si>
+  <si>
+    <t>Line Driver</t>
+  </si>
+  <si>
+    <t>ARC-H-50-3600-HTL-6-3M-FZ</t>
+  </si>
+  <si>
+    <t>TTL</t>
   </si>
 </sst>
 </file>
@@ -547,24 +547,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,17 +578,20 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -598,20 +602,23 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="19">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="19">
         <v>250</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="16">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -624,17 +631,23 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="19">
         <v>117</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="16">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -647,199 +660,206 @@
       <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="G4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="12"/>
       <c r="C6" s="14"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="4"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="11"/>
       <c r="C7" s="14"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="12"/>
       <c r="C8" s="14"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="12"/>
       <c r="C9" s="14"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="12"/>
       <c r="C10" s="14"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="12"/>
       <c r="C11" s="14"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="12"/>
       <c r="C12" s="14"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="12"/>
       <c r="C13" s="14"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="12"/>
       <c r="C14" s="14"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="12"/>
       <c r="C15" s="14"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="12"/>
       <c r="C16" s="14"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="12"/>
       <c r="C17" s="14"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="12"/>
       <c r="C18" s="14"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="4"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="12"/>
       <c r="C19" s="14"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="16">
+      <c r="E19" s="4"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="16">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" location="/besleme_gerilimi-5_30vdc/k_devresi-abztersleri/balant_ekli-2mt_kablolu/gvde_ap-100mm/delik_ap-23mm/puls-5000 "/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" location="/besleme_gerilimi-5_30vdc/k_devresi-abztersleri/balant_ekli-2mt_kablolu/gvde_ap-100mm/delik_ap-23mm/puls-5000 "/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The overshoot magnitudes are corrected. However, the oscillations don't damp now. Backward Euler Integration method is implemented.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/IMMD Production/Encoder.xlsx
+++ b/Project/3501/Furkan/IMMD Production/Encoder.xlsx
@@ -96,10 +96,10 @@
     <t>Line Driver</t>
   </si>
   <si>
-    <t>ARC-H-50-3600-HTL-6-3M-FZ</t>
-  </si>
-  <si>
     <t>TTL</t>
+  </si>
+  <si>
+    <t>ARC-H-50-3600-TTL-6-3M-10-FC</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="19">
         <v>117</v>
@@ -644,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>